<commit_message>
Context Classe, ClasseHabilidade e Personagem feitas
</commit_message>
<xml_diff>
--- a/HROADS-SENAI/modelagem-HROADS/Hroads-modelagem-fisico.xlsx
+++ b/HROADS-SENAI/modelagem-HROADS/Hroads-modelagem-fisico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Desktop\Senai_Hroads_API_2DT\HROADS-SENAI\modelagem-HROADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8CEC8D-A0A4-4986-9879-49170306CFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E277839-B558-4482-9ECF-6BDEDEB0C3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4485" yWindow="990" windowWidth="15375" windowHeight="7875" xr2:uid="{5B9D3288-11C5-40DE-97AF-AFB42676E53E}"/>
+    <workbookView minimized="1" xWindow="4830" yWindow="1335" windowWidth="15375" windowHeight="7875" xr2:uid="{5B9D3288-11C5-40DE-97AF-AFB42676E53E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>tipoHabilidade</t>
   </si>
@@ -130,18 +130,6 @@
   </si>
   <si>
     <t>idClasseHabilidade</t>
-  </si>
-  <si>
-    <t>Classe</t>
-  </si>
-  <si>
-    <t>NomePersonagem</t>
-  </si>
-  <si>
-    <t>capacidadeDeVidaMax</t>
-  </si>
-  <si>
-    <t>capacidadeDeManaMax</t>
   </si>
 </sst>
 </file>
@@ -770,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03624503-7B4D-416C-8BB8-14BA7E7934D4}">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>28</v>
@@ -1092,7 +1080,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>29</v>
@@ -1119,8 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1137,10 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1157,10 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1177,10 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="J20" s="29">
         <v>4</v>
       </c>
@@ -1191,10 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
-        <v>37</v>
-      </c>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="J21" s="28">
         <v>5</v>
       </c>
@@ -1206,10 +1181,7 @@
       </c>
       <c r="M21" s="25"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
-        <v>38</v>
-      </c>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="J22" s="28">
         <v>6</v>
       </c>
@@ -1220,10 +1192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
-        <v>11</v>
-      </c>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="J23" s="28">
         <v>7</v>
       </c>
@@ -1232,11 +1201,6 @@
       </c>
       <c r="L23" s="28">
         <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>